<commit_message>
FEATURE: Interest Rates Update
</commit_message>
<xml_diff>
--- a/src/currentCurrencyTrades/assets/report.xlsx
+++ b/src/currentCurrencyTrades/assets/report.xlsx
@@ -49,10 +49,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Could not fetch the exchange Rates, the url is https://www.bancomoc.mz/Files/REFR/ZMIREFR.pdf</t>
-  </si>
-  <si>
-    <t>2022-09-04 22:32:28</t>
+    <t>Coould not fetch interest Rates. Invalid date 2022-09-05, valid date format exemple: 05/09/2022</t>
+  </si>
+  <si>
+    <t>2022-09-05 21:18:10</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
IMPROVE: Schedule and jobs
</commit_message>
<xml_diff>
--- a/src/currentCurrencyTrades/assets/report.xlsx
+++ b/src/currentCurrencyTrades/assets/report.xlsx
@@ -49,10 +49,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Was not able to save the task of CPI.</t>
-  </si>
-  <si>
-    <t>2022-09-22 11:56:50</t>
+    <t>Was not able to save the task of exchange rates.</t>
+  </si>
+  <si>
+    <t>2022-09-26 12:39:49</t>
   </si>
 </sst>
 </file>

</xml_diff>